<commit_message>
luego de mucho tiempo
</commit_message>
<xml_diff>
--- a/PUNTOS FINALES.xlsx
+++ b/PUNTOS FINALES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leine\Documentos\QUINIELA-VENECA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D022090-3ABC-415F-9BE6-A1DA9695E304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABAD2555-BD5A-4B20-98DE-976219C0E490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{14857883-2667-4317-B409-2C4B62DE3E70}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{14857883-2667-4317-B409-2C4B62DE3E70}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -496,7 +496,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,14 +638,14 @@
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="E7" s="6"/>
       <c r="F7" s="5"/>
       <c r="G7" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" si="0"/>
-        <v>385.01299999999998</v>
+        <v>395.01299999999998</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -714,14 +714,14 @@
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="6"/>
+      <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H11" s="2">
         <f t="shared" si="0"/>
-        <v>355.012</v>
+        <v>345.012</v>
       </c>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.25">

</xml_diff>